<commit_message>
TOR-016 New Band Implementation - Refactor character and band classes; introduce Game and GameFactory services
- Removed legacy CharacterTOR and BandTOR classes, replacing them with new implementations in TheOneRingDetails.
- Created Game and GameFactory classes to manage game state and asset selection.
- Added BandTORLoader for loading band data from Excel.
- Introduced GameTORService for static utility methods related to game configuration.
- Updated main application to utilize new Game and GameTOR classes for asset management.
- Enhanced ally management within BandTOR, including injury and fatigue tracking.
- Updated requirements.txt for dependency management.
</commit_message>
<xml_diff>
--- a/data/Band.xlsx
+++ b/data/Band.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">hardened</t>
   </si>
   <si>
-    <t xml:space="preserve">gift </t>
+    <t xml:space="preserve">gift</t>
   </si>
   <si>
     <t xml:space="preserve">giftWasted</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">kinglyGiftWasted</t>
   </si>
   <si>
-    <t xml:space="preserve">quirksOrNotes </t>
+    <t xml:space="preserve">quirksOrNotes</t>
   </si>
   <si>
     <t xml:space="preserve">Dúrnir</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">Licha bródka zdobi młodociane oblicze</t>
   </si>
   <si>
-    <t xml:space="preserve">Galar - Słuchający Skały</t>
+    <t xml:space="preserve">Galar</t>
   </si>
   <si>
     <t xml:space="preserve">ZŁODZIEJASZEK</t>
@@ -160,7 +160,7 @@
   <si>
     <t xml:space="preserve">Tarczę zdobi wojennymi trofeami:
 - Pot. pod Aleją Królów
-- Ekstrakcja inż. Eiri'ego
+- Ekstrakcja inż. Eitri'ego
 Walczy włócznią z tarczą</t>
   </si>
   <si>
@@ -253,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,6 +263,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,7 +294,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,13 +329,13 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -352,7 +356,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>14</v>
@@ -360,13 +364,13 @@
       <c r="H2" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="J2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -408,14 +412,14 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="32.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="32.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,16 +482,19 @@
       <c r="G2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -513,16 +520,19 @@
       <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -554,10 +564,13 @@
       <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -589,10 +602,13 @@
       <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -624,14 +640,17 @@
       <c r="I6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="K6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -658,6 +677,9 @@
       </c>
       <c r="I7" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>28</v>
@@ -693,6 +715,9 @@
       </c>
       <c r="I8" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
TOR-21 Impl interaction between Hero and Treasury
Implement:
- RecordSaver
- HeroTOR
- ItemTOR,
- Upgrade related services eg Game and Band
</commit_message>
<xml_diff>
--- a/data/Band.xlsx
+++ b/data/Band.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bands" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Allies" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Heroes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Allies" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Items" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -65,7 +67,13 @@
     <t xml:space="preserve">MEDIUM</t>
   </si>
   <si>
-    <t xml:space="preserve">EXPERTISE</t>
+    <t xml:space="preserve">VIGILANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qwer1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veig</t>
   </si>
   <si>
     <t xml:space="preserve">idBand</t>
@@ -168,6 +176,48 @@
   </si>
   <si>
     <t xml:space="preserve">INŻYNIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idOwner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benefit1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">benefit2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isCursed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sword of Destiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A legendary sword with a glowing blade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ItemSlotTypeTOR.WEAPON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SkillTypeTOR.BATTLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SkillTypeTOR.NONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MagicItemType.UNUSUAL</t>
   </si>
 </sst>
 </file>
@@ -253,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +314,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -293,8 +347,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,16 +413,16 @@
         <v>3</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>0</v>
@@ -409,17 +463,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="32.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="32.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,37 +524,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,34 +565,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>30</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,34 +603,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,34 +641,34 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,34 +679,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,34 +717,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -658,34 +755,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,31 +793,113 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TOR-23 Fix sheet Band/Hero
</commit_message>
<xml_diff>
--- a/data/Band.xlsx
+++ b/data/Band.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -208,16 +208,13 @@
     <t xml:space="preserve">A legendary sword with a glowing blade.</t>
   </si>
   <si>
-    <t xml:space="preserve">ItemSlotTypeTOR.WEAPON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SkillTypeTOR.BATTLE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SkillTypeTOR.NONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MagicItemType.UNUSUAL</t>
+    <t xml:space="preserve">WEAPON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNUSUAL</t>
   </si>
 </sst>
 </file>
@@ -839,7 +836,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -893,13 +890,13 @@
         <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>